<commit_message>
Improved layout of table with user defined column width and cenered bold table headers
</commit_message>
<xml_diff>
--- a/src_data.xlsx
+++ b/src_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sacha\python files\Small Projects\01. Populate MS Word from DB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sacha\python files\Small Projects\01. Populate MS Word from DB\database_to_word\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC10BA75-47D0-445D-AA41-1D90AEEE1A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463F716F-626C-4641-AE4D-28C7DCDA740C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6FC0E80D-A453-475C-9F3B-9FC652769436}"/>
   </bookViews>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>number</t>
   </si>
@@ -50,25 +39,13 @@
     <t>Initiation</t>
   </si>
   <si>
-    <t>Opinion on MDP</t>
-  </si>
-  <si>
     <t>model_development</t>
   </si>
   <si>
     <t>model_validation</t>
   </si>
   <si>
-    <t>Build Model</t>
-  </si>
-  <si>
     <t>Development</t>
-  </si>
-  <si>
-    <t>kill the model</t>
-  </si>
-  <si>
-    <t>talk to each other</t>
   </si>
   <si>
     <t>Retirement</t>
@@ -76,6 +53,78 @@
   <si>
     <t>write MDP. We need a lot of text to see what it will look like in a table. Test the layout and potentatially adjust
 - another line</t>
+  </si>
+  <si>
+    <t>MRP 1.1</t>
+  </si>
+  <si>
+    <t>topic</t>
+  </si>
+  <si>
+    <t>Objective</t>
+  </si>
+  <si>
+    <t>MRP 1.2</t>
+  </si>
+  <si>
+    <t>Planning</t>
+  </si>
+  <si>
+    <t>Make a planning</t>
+  </si>
+  <si>
+    <t>MRP 2.1</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>Model needs a purpose</t>
+  </si>
+  <si>
+    <t>MRP 2.2</t>
+  </si>
+  <si>
+    <t>Document</t>
+  </si>
+  <si>
+    <t>Model results needs to be documented</t>
+  </si>
+  <si>
+    <t>MRP 3.1</t>
+  </si>
+  <si>
+    <t>Validation</t>
+  </si>
+  <si>
+    <t>Model needs to be validated</t>
+  </si>
+  <si>
+    <t>MRP 4.1</t>
+  </si>
+  <si>
+    <t>Model needs to be implemented</t>
+  </si>
+  <si>
+    <t>Implementation</t>
+  </si>
+  <si>
+    <t>MRP 5.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use </t>
+  </si>
+  <si>
+    <t>Users need to understand the model</t>
+  </si>
+  <si>
+    <t>Use</t>
+  </si>
+  <si>
+    <t>MRP 6.1</t>
+  </si>
+  <si>
+    <t>Model needs to be turned off</t>
   </si>
 </sst>
 </file>
@@ -430,118 +479,196 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1C4AB8C-5A0A-414C-A916-E4DA37E829A1}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="46.21875" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" customWidth="1"/>
-    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.21875" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="b">
-        <v>1</v>
-      </c>
-      <c r="E5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="b">
-        <v>1</v>
-      </c>
-      <c r="E6" t="b">
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>